<commit_message>
Merge klaar met veranderingen.
</commit_message>
<xml_diff>
--- a/SprintPlannerZM.Ui.Mvc/ExamenPerLeerling.xlsx
+++ b/SprintPlannerZM.Ui.Mvc/ExamenPerLeerling.xlsx
@@ -14,7 +14,65 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <x:si>
+    <x:t>1A1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Maité Bonte</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Datum</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Uur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Soort</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Proefwerk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lokaal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10:25:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sprint</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Engels-1u</x:t>
+  </x:si>
+  <x:si>
+    <x:t>biep!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Frans-3u</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Godsdienst</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Esther Bovée</x:t>
+  </x:si>
+  <x:si>
+    <x:t>typer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lea Caerels</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mklas</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8:30:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Aardrijkskunde-2u</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22,8 +80,17 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:u val="single"/>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
@@ -39,7 +106,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="1">
+  <x:borders count="2">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -57,15 +124,65 @@
         <x:color rgb="FF000000"/>
       </x:diagonal>
     </x:border>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="thick">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -363,7 +480,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:E78"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -375,7 +492,671 @@
     <x:col min="4" max="4" width="40.710625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="10.710625" style="0" customWidth="1"/>
   </x:cols>
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A1" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s"/>
+      <x:c r="D1" s="1" t="s"/>
+      <x:c r="E1" s="1" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A3" s="4">
+        <x:v>44279</x:v>
+      </x:c>
+      <x:c r="B3" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="5" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D3" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E3" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A4" s="4">
+        <x:v>44280</x:v>
+      </x:c>
+      <x:c r="B4" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C4" s="5" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D4" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E4" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A5" s="4">
+        <x:v>44284</x:v>
+      </x:c>
+      <x:c r="B5" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C5" s="5" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D5" s="5" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="E5" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A6" s="6" t="s"/>
+      <x:c r="B6" s="5" t="s"/>
+      <x:c r="C6" s="5" t="s"/>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="E6" s="6" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A7" s="6" t="s"/>
+      <x:c r="B7" s="5" t="s"/>
+      <x:c r="C7" s="5" t="s"/>
+      <x:c r="D7" s="5" t="s"/>
+      <x:c r="E7" s="6" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A8" s="6" t="s"/>
+      <x:c r="B8" s="5" t="s"/>
+      <x:c r="C8" s="5" t="s"/>
+      <x:c r="D8" s="5" t="s"/>
+      <x:c r="E8" s="6" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A9" s="6" t="s"/>
+      <x:c r="B9" s="5" t="s"/>
+      <x:c r="C9" s="5" t="s"/>
+      <x:c r="D9" s="5" t="s"/>
+      <x:c r="E9" s="6" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A10" s="6" t="s"/>
+      <x:c r="B10" s="5" t="s"/>
+      <x:c r="C10" s="5" t="s"/>
+      <x:c r="D10" s="5" t="s"/>
+      <x:c r="E10" s="6" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="5" t="s"/>
+      <x:c r="C11" s="5" t="s"/>
+      <x:c r="D11" s="5" t="s"/>
+      <x:c r="E11" s="6" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="5" t="s"/>
+      <x:c r="C12" s="5" t="s"/>
+      <x:c r="D12" s="5" t="s"/>
+      <x:c r="E12" s="6" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A13" s="6" t="s"/>
+      <x:c r="B13" s="5" t="s"/>
+      <x:c r="C13" s="5" t="s"/>
+      <x:c r="D13" s="5" t="s"/>
+      <x:c r="E13" s="6" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A14" s="6" t="s"/>
+      <x:c r="B14" s="5" t="s"/>
+      <x:c r="C14" s="5" t="s"/>
+      <x:c r="D14" s="5" t="s"/>
+      <x:c r="E14" s="6" t="s"/>
+    </x:row>
+    <x:row r="15" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A15" s="6" t="s"/>
+      <x:c r="B15" s="5" t="s"/>
+      <x:c r="C15" s="5" t="s"/>
+      <x:c r="D15" s="5" t="s"/>
+      <x:c r="E15" s="6" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A16" s="6" t="s"/>
+      <x:c r="B16" s="5" t="s"/>
+      <x:c r="C16" s="5" t="s"/>
+      <x:c r="D16" s="5" t="s"/>
+      <x:c r="E16" s="6" t="s"/>
+    </x:row>
+    <x:row r="17" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A17" s="6" t="s"/>
+      <x:c r="B17" s="5" t="s"/>
+      <x:c r="C17" s="5" t="s"/>
+      <x:c r="D17" s="5" t="s"/>
+      <x:c r="E17" s="6" t="s"/>
+    </x:row>
+    <x:row r="18" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A18" s="6" t="s"/>
+      <x:c r="B18" s="5" t="s"/>
+      <x:c r="C18" s="5" t="s"/>
+      <x:c r="D18" s="5" t="s"/>
+      <x:c r="E18" s="6" t="s"/>
+    </x:row>
+    <x:row r="19" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A19" s="6" t="s"/>
+      <x:c r="B19" s="5" t="s"/>
+      <x:c r="C19" s="5" t="s"/>
+      <x:c r="D19" s="5" t="s"/>
+      <x:c r="E19" s="6" t="s"/>
+    </x:row>
+    <x:row r="20" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A20" s="6" t="s"/>
+      <x:c r="B20" s="5" t="s"/>
+      <x:c r="C20" s="5" t="s"/>
+      <x:c r="D20" s="5" t="s"/>
+      <x:c r="E20" s="6" t="s"/>
+    </x:row>
+    <x:row r="21" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A21" s="6" t="s"/>
+      <x:c r="B21" s="5" t="s"/>
+      <x:c r="C21" s="5" t="s"/>
+      <x:c r="D21" s="5" t="s"/>
+      <x:c r="E21" s="6" t="s"/>
+    </x:row>
+    <x:row r="22" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A22" s="6" t="s"/>
+      <x:c r="B22" s="5" t="s"/>
+      <x:c r="C22" s="5" t="s"/>
+      <x:c r="D22" s="5" t="s"/>
+      <x:c r="E22" s="6" t="s"/>
+    </x:row>
+    <x:row r="23" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A23" s="6" t="s"/>
+      <x:c r="B23" s="5" t="s"/>
+      <x:c r="C23" s="5" t="s"/>
+      <x:c r="D23" s="5" t="s"/>
+      <x:c r="E23" s="6" t="s"/>
+    </x:row>
+    <x:row r="24" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A24" s="6" t="s"/>
+      <x:c r="B24" s="5" t="s"/>
+      <x:c r="C24" s="5" t="s"/>
+      <x:c r="D24" s="5" t="s"/>
+      <x:c r="E24" s="6" t="s"/>
+    </x:row>
+    <x:row r="25" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A25" s="6" t="s"/>
+      <x:c r="B25" s="5" t="s"/>
+      <x:c r="C25" s="5" t="s"/>
+      <x:c r="D25" s="5" t="s"/>
+      <x:c r="E25" s="6" t="s"/>
+    </x:row>
+    <x:row r="26" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A26" s="6" t="s"/>
+      <x:c r="B26" s="5" t="s"/>
+      <x:c r="C26" s="5" t="s"/>
+      <x:c r="D26" s="5" t="s"/>
+      <x:c r="E26" s="6" t="s"/>
+    </x:row>
+    <x:row r="27" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A27" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B27" s="1" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C27" s="1" t="s"/>
+      <x:c r="D27" s="1" t="s"/>
+      <x:c r="E27" s="1" t="s"/>
+    </x:row>
+    <x:row r="28" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A28" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B28" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C28" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D28" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E28" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A29" s="4">
+        <x:v>44279</x:v>
+      </x:c>
+      <x:c r="B29" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C29" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D29" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E29" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A30" s="4">
+        <x:v>44280</x:v>
+      </x:c>
+      <x:c r="B30" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C30" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D30" s="5" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="E30" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A31" s="6" t="s"/>
+      <x:c r="B31" s="5" t="s"/>
+      <x:c r="C31" s="5" t="s"/>
+      <x:c r="D31" s="5" t="s"/>
+      <x:c r="E31" s="6" t="s"/>
+    </x:row>
+    <x:row r="32" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A32" s="6" t="s"/>
+      <x:c r="B32" s="5" t="s"/>
+      <x:c r="C32" s="5" t="s"/>
+      <x:c r="D32" s="5" t="s"/>
+      <x:c r="E32" s="6" t="s"/>
+    </x:row>
+    <x:row r="33" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A33" s="6" t="s"/>
+      <x:c r="B33" s="5" t="s"/>
+      <x:c r="C33" s="5" t="s"/>
+      <x:c r="D33" s="5" t="s"/>
+      <x:c r="E33" s="6" t="s"/>
+    </x:row>
+    <x:row r="34" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A34" s="6" t="s"/>
+      <x:c r="B34" s="5" t="s"/>
+      <x:c r="C34" s="5" t="s"/>
+      <x:c r="D34" s="5" t="s"/>
+      <x:c r="E34" s="6" t="s"/>
+    </x:row>
+    <x:row r="35" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A35" s="6" t="s"/>
+      <x:c r="B35" s="5" t="s"/>
+      <x:c r="C35" s="5" t="s"/>
+      <x:c r="D35" s="5" t="s"/>
+      <x:c r="E35" s="6" t="s"/>
+    </x:row>
+    <x:row r="36" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A36" s="6" t="s"/>
+      <x:c r="B36" s="5" t="s"/>
+      <x:c r="C36" s="5" t="s"/>
+      <x:c r="D36" s="5" t="s"/>
+      <x:c r="E36" s="6" t="s"/>
+    </x:row>
+    <x:row r="37" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A37" s="6" t="s"/>
+      <x:c r="B37" s="5" t="s"/>
+      <x:c r="C37" s="5" t="s"/>
+      <x:c r="D37" s="5" t="s"/>
+      <x:c r="E37" s="6" t="s"/>
+    </x:row>
+    <x:row r="38" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A38" s="6" t="s"/>
+      <x:c r="B38" s="5" t="s"/>
+      <x:c r="C38" s="5" t="s"/>
+      <x:c r="D38" s="5" t="s"/>
+      <x:c r="E38" s="6" t="s"/>
+    </x:row>
+    <x:row r="39" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A39" s="6" t="s"/>
+      <x:c r="B39" s="5" t="s"/>
+      <x:c r="C39" s="5" t="s"/>
+      <x:c r="D39" s="5" t="s"/>
+      <x:c r="E39" s="6" t="s"/>
+    </x:row>
+    <x:row r="40" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A40" s="6" t="s"/>
+      <x:c r="B40" s="5" t="s"/>
+      <x:c r="C40" s="5" t="s"/>
+      <x:c r="D40" s="5" t="s"/>
+      <x:c r="E40" s="6" t="s"/>
+    </x:row>
+    <x:row r="41" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A41" s="6" t="s"/>
+      <x:c r="B41" s="5" t="s"/>
+      <x:c r="C41" s="5" t="s"/>
+      <x:c r="D41" s="5" t="s"/>
+      <x:c r="E41" s="6" t="s"/>
+    </x:row>
+    <x:row r="42" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A42" s="6" t="s"/>
+      <x:c r="B42" s="5" t="s"/>
+      <x:c r="C42" s="5" t="s"/>
+      <x:c r="D42" s="5" t="s"/>
+      <x:c r="E42" s="6" t="s"/>
+    </x:row>
+    <x:row r="43" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A43" s="6" t="s"/>
+      <x:c r="B43" s="5" t="s"/>
+      <x:c r="C43" s="5" t="s"/>
+      <x:c r="D43" s="5" t="s"/>
+      <x:c r="E43" s="6" t="s"/>
+    </x:row>
+    <x:row r="44" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A44" s="6" t="s"/>
+      <x:c r="B44" s="5" t="s"/>
+      <x:c r="C44" s="5" t="s"/>
+      <x:c r="D44" s="5" t="s"/>
+      <x:c r="E44" s="6" t="s"/>
+    </x:row>
+    <x:row r="45" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A45" s="6" t="s"/>
+      <x:c r="B45" s="5" t="s"/>
+      <x:c r="C45" s="5" t="s"/>
+      <x:c r="D45" s="5" t="s"/>
+      <x:c r="E45" s="6" t="s"/>
+    </x:row>
+    <x:row r="46" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A46" s="6" t="s"/>
+      <x:c r="B46" s="5" t="s"/>
+      <x:c r="C46" s="5" t="s"/>
+      <x:c r="D46" s="5" t="s"/>
+      <x:c r="E46" s="6" t="s"/>
+    </x:row>
+    <x:row r="47" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A47" s="6" t="s"/>
+      <x:c r="B47" s="5" t="s"/>
+      <x:c r="C47" s="5" t="s"/>
+      <x:c r="D47" s="5" t="s"/>
+      <x:c r="E47" s="6" t="s"/>
+    </x:row>
+    <x:row r="48" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A48" s="6" t="s"/>
+      <x:c r="B48" s="5" t="s"/>
+      <x:c r="C48" s="5" t="s"/>
+      <x:c r="D48" s="5" t="s"/>
+      <x:c r="E48" s="6" t="s"/>
+    </x:row>
+    <x:row r="49" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A49" s="6" t="s"/>
+      <x:c r="B49" s="5" t="s"/>
+      <x:c r="C49" s="5" t="s"/>
+      <x:c r="D49" s="5" t="s"/>
+      <x:c r="E49" s="6" t="s"/>
+    </x:row>
+    <x:row r="50" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A50" s="6" t="s"/>
+      <x:c r="B50" s="5" t="s"/>
+      <x:c r="C50" s="5" t="s"/>
+      <x:c r="D50" s="5" t="s"/>
+      <x:c r="E50" s="6" t="s"/>
+    </x:row>
+    <x:row r="51" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A51" s="6" t="s"/>
+      <x:c r="B51" s="5" t="s"/>
+      <x:c r="C51" s="5" t="s"/>
+      <x:c r="D51" s="5" t="s"/>
+      <x:c r="E51" s="6" t="s"/>
+    </x:row>
+    <x:row r="52" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A52" s="6" t="s"/>
+      <x:c r="B52" s="5" t="s"/>
+      <x:c r="C52" s="5" t="s"/>
+      <x:c r="D52" s="5" t="s"/>
+      <x:c r="E52" s="6" t="s"/>
+    </x:row>
+    <x:row r="53" spans="1:5" s="1" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A53" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B53" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C53" s="1" t="s"/>
+      <x:c r="D53" s="1" t="s"/>
+      <x:c r="E53" s="1" t="s"/>
+    </x:row>
+    <x:row r="54" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A54" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B54" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C54" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D54" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E54" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A55" s="4">
+        <x:v>44279</x:v>
+      </x:c>
+      <x:c r="B55" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C55" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D55" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E55" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="56" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A56" s="4">
+        <x:v>44280</x:v>
+      </x:c>
+      <x:c r="B56" s="5" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="C56" s="5" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D56" s="5" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E56" s="6" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="57" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A57" s="6" t="s"/>
+      <x:c r="B57" s="5" t="s"/>
+      <x:c r="C57" s="5" t="s"/>
+      <x:c r="D57" s="5" t="s"/>
+      <x:c r="E57" s="6" t="s"/>
+    </x:row>
+    <x:row r="58" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A58" s="6" t="s"/>
+      <x:c r="B58" s="5" t="s"/>
+      <x:c r="C58" s="5" t="s"/>
+      <x:c r="D58" s="5" t="s"/>
+      <x:c r="E58" s="6" t="s"/>
+    </x:row>
+    <x:row r="59" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A59" s="6" t="s"/>
+      <x:c r="B59" s="5" t="s"/>
+      <x:c r="C59" s="5" t="s"/>
+      <x:c r="D59" s="5" t="s"/>
+      <x:c r="E59" s="6" t="s"/>
+    </x:row>
+    <x:row r="60" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A60" s="6" t="s"/>
+      <x:c r="B60" s="5" t="s"/>
+      <x:c r="C60" s="5" t="s"/>
+      <x:c r="D60" s="5" t="s"/>
+      <x:c r="E60" s="6" t="s"/>
+    </x:row>
+    <x:row r="61" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A61" s="6" t="s"/>
+      <x:c r="B61" s="5" t="s"/>
+      <x:c r="C61" s="5" t="s"/>
+      <x:c r="D61" s="5" t="s"/>
+      <x:c r="E61" s="6" t="s"/>
+    </x:row>
+    <x:row r="62" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A62" s="6" t="s"/>
+      <x:c r="B62" s="5" t="s"/>
+      <x:c r="C62" s="5" t="s"/>
+      <x:c r="D62" s="5" t="s"/>
+      <x:c r="E62" s="6" t="s"/>
+    </x:row>
+    <x:row r="63" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A63" s="6" t="s"/>
+      <x:c r="B63" s="5" t="s"/>
+      <x:c r="C63" s="5" t="s"/>
+      <x:c r="D63" s="5" t="s"/>
+      <x:c r="E63" s="6" t="s"/>
+    </x:row>
+    <x:row r="64" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A64" s="6" t="s"/>
+      <x:c r="B64" s="5" t="s"/>
+      <x:c r="C64" s="5" t="s"/>
+      <x:c r="D64" s="5" t="s"/>
+      <x:c r="E64" s="6" t="s"/>
+    </x:row>
+    <x:row r="65" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A65" s="6" t="s"/>
+      <x:c r="B65" s="5" t="s"/>
+      <x:c r="C65" s="5" t="s"/>
+      <x:c r="D65" s="5" t="s"/>
+      <x:c r="E65" s="6" t="s"/>
+    </x:row>
+    <x:row r="66" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A66" s="6" t="s"/>
+      <x:c r="B66" s="5" t="s"/>
+      <x:c r="C66" s="5" t="s"/>
+      <x:c r="D66" s="5" t="s"/>
+      <x:c r="E66" s="6" t="s"/>
+    </x:row>
+    <x:row r="67" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A67" s="6" t="s"/>
+      <x:c r="B67" s="5" t="s"/>
+      <x:c r="C67" s="5" t="s"/>
+      <x:c r="D67" s="5" t="s"/>
+      <x:c r="E67" s="6" t="s"/>
+    </x:row>
+    <x:row r="68" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A68" s="6" t="s"/>
+      <x:c r="B68" s="5" t="s"/>
+      <x:c r="C68" s="5" t="s"/>
+      <x:c r="D68" s="5" t="s"/>
+      <x:c r="E68" s="6" t="s"/>
+    </x:row>
+    <x:row r="69" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A69" s="6" t="s"/>
+      <x:c r="B69" s="5" t="s"/>
+      <x:c r="C69" s="5" t="s"/>
+      <x:c r="D69" s="5" t="s"/>
+      <x:c r="E69" s="6" t="s"/>
+    </x:row>
+    <x:row r="70" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A70" s="6" t="s"/>
+      <x:c r="B70" s="5" t="s"/>
+      <x:c r="C70" s="5" t="s"/>
+      <x:c r="D70" s="5" t="s"/>
+      <x:c r="E70" s="6" t="s"/>
+    </x:row>
+    <x:row r="71" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A71" s="6" t="s"/>
+      <x:c r="B71" s="5" t="s"/>
+      <x:c r="C71" s="5" t="s"/>
+      <x:c r="D71" s="5" t="s"/>
+      <x:c r="E71" s="6" t="s"/>
+    </x:row>
+    <x:row r="72" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A72" s="6" t="s"/>
+      <x:c r="B72" s="5" t="s"/>
+      <x:c r="C72" s="5" t="s"/>
+      <x:c r="D72" s="5" t="s"/>
+      <x:c r="E72" s="6" t="s"/>
+    </x:row>
+    <x:row r="73" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A73" s="6" t="s"/>
+      <x:c r="B73" s="5" t="s"/>
+      <x:c r="C73" s="5" t="s"/>
+      <x:c r="D73" s="5" t="s"/>
+      <x:c r="E73" s="6" t="s"/>
+    </x:row>
+    <x:row r="74" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A74" s="6" t="s"/>
+      <x:c r="B74" s="5" t="s"/>
+      <x:c r="C74" s="5" t="s"/>
+      <x:c r="D74" s="5" t="s"/>
+      <x:c r="E74" s="6" t="s"/>
+    </x:row>
+    <x:row r="75" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A75" s="6" t="s"/>
+      <x:c r="B75" s="5" t="s"/>
+      <x:c r="C75" s="5" t="s"/>
+      <x:c r="D75" s="5" t="s"/>
+      <x:c r="E75" s="6" t="s"/>
+    </x:row>
+    <x:row r="76" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A76" s="6" t="s"/>
+      <x:c r="B76" s="5" t="s"/>
+      <x:c r="C76" s="5" t="s"/>
+      <x:c r="D76" s="5" t="s"/>
+      <x:c r="E76" s="6" t="s"/>
+    </x:row>
+    <x:row r="77" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A77" s="6" t="s"/>
+      <x:c r="B77" s="5" t="s"/>
+      <x:c r="C77" s="5" t="s"/>
+      <x:c r="D77" s="5" t="s"/>
+      <x:c r="E77" s="6" t="s"/>
+    </x:row>
+    <x:row r="78" spans="1:5" customFormat="1" ht="20" customHeight="1">
+      <x:c r="A78" s="6" t="s"/>
+      <x:c r="B78" s="5" t="s"/>
+      <x:c r="C78" s="5" t="s"/>
+      <x:c r="D78" s="5" t="s"/>
+      <x:c r="E78" s="6" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells count="3">
+    <x:mergeCell ref="B1:E1"/>
+    <x:mergeCell ref="B27:E27"/>
+    <x:mergeCell ref="B53:E53"/>
+  </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="landscape" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>